<commit_message>
Revert "Actualizacion Excel Juan"
This reverts commit c17c8bb4a53dd0c5a0209a5b3685dcdfab516bf5.
</commit_message>
<xml_diff>
--- a/control de tareas Unidad II - Juan.xlsx
+++ b/control de tareas Unidad II - Juan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdalbertoPc\Documents\luterano 2016\Bachillerato\tareas\videosDigital\PunteosActividades5to\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="8820" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="8820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Creacion de canal de Youtube" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +66,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +91,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +116,7 @@
     <author>AdalbertoPc</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>hoja de cotejo Produccion de Contenidos digitales.</t>
   </si>
@@ -260,15 +265,12 @@
   </si>
   <si>
     <t>Julio</t>
-  </si>
-  <si>
-    <t>Luis Mendez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,7 +526,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -576,7 +578,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -770,7 +772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -784,12 +786,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -801,7 +803,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
@@ -809,7 +811,7 @@
         <v>42467</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -826,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -841,7 +843,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -856,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -871,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -886,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -901,7 +903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -916,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -925,7 +927,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -954,13 +956,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="4"/>
+    <col min="1" max="1" width="4.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -972,7 +974,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
@@ -980,14 +982,14 @@
         <v>42481</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1021,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1051,7 +1053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1090,7 +1092,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1099,7 +1101,7 @@
       <c r="D13" s="13"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>8</v>
       </c>
@@ -1123,17 +1125,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="4"/>
+    <col min="3" max="3" width="30.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -1145,7 +1147,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
@@ -1153,14 +1155,14 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1187,14 +1189,12 @@
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1202,14 +1202,12 @@
       <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="D8" s="13"/>
       <c r="E8" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1217,14 +1215,12 @@
       <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -1232,14 +1228,12 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1247,14 +1241,12 @@
       <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1263,7 +1255,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1272,7 +1264,7 @@
       <c r="D13" s="13"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>8</v>
       </c>
@@ -1296,20 +1288,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="4" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="4"/>
+    <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1310,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
@@ -1326,14 +1318,14 @@
         <v>42509</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1350,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1360,12 +1352,10 @@
       <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1373,12 +1363,10 @@
       <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="D8" s="13"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1386,12 +1374,10 @@
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -1399,12 +1385,10 @@
       <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1412,12 +1396,10 @@
       <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1426,7 +1408,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1435,7 +1417,7 @@
       <c r="D13" s="13"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>8</v>
       </c>

</xml_diff>